<commit_message>
first recorded check, creating columns for every document that needs to be checked.
</commit_message>
<xml_diff>
--- a/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Dokumente.xlsx
+++ b/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Dokumente.xlsx
@@ -84,13 +84,13 @@
     <t>Architekturdokument</t>
   </si>
   <si>
-    <t>Projekthandbuch</t>
-  </si>
-  <si>
     <t>Anforderungsdokument</t>
   </si>
   <si>
     <t>Testreport(?)</t>
+  </si>
+  <si>
+    <t>Installationsanleitung</t>
   </si>
 </sst>
 </file>
@@ -435,14 +435,14 @@
   <dimension ref="B1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -456,13 +456,13 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="2:7">

</xml_diff>

<commit_message>
new checklist for the installation manual, fixed one checkpoint in the genereic document checklist
</commit_message>
<xml_diff>
--- a/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Dokumente.xlsx
+++ b/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Dokumente.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Checkliste Dokumente</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Abbildungsbeschriftungen vorhanden und sinnvoll?</t>
   </si>
   <si>
-    <t>Leere Füllseiten im Dokument?</t>
-  </si>
-  <si>
     <t>Zu jedem Diagramm/Abbildung eine Beschreibung vorhanden?</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>ja</t>
   </si>
   <si>
-    <t>nein</t>
-  </si>
-  <si>
     <t>Tabellenbeschriftungen vorhanden und sinnvoll?</t>
   </si>
   <si>
@@ -91,6 +85,9 @@
   </si>
   <si>
     <t>Installationsanleitung</t>
+  </si>
+  <si>
+    <t>Alle Seiten mit sinnvollem Inhalt gefüllt?</t>
   </si>
 </sst>
 </file>
@@ -435,7 +432,7 @@
   <dimension ref="B1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -453,24 +450,24 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:7">
@@ -478,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -486,15 +483,15 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -502,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:7">
@@ -510,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:7">
@@ -518,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:7">
@@ -526,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:7">
@@ -534,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:7">
@@ -542,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:7">
@@ -550,15 +547,15 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:7">
@@ -566,15 +563,15 @@
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -582,22 +579,22 @@
         <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:5">

</xml_diff>

<commit_message>
checked user stories final document and installation manual, reported improvement advice to dweidle
</commit_message>
<xml_diff>
--- a/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Dokumente.xlsx
+++ b/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Dokumente.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
   <si>
     <t>Checkliste Dokumente</t>
   </si>
@@ -78,16 +78,37 @@
     <t>Architekturdokument</t>
   </si>
   <si>
-    <t>Anforderungsdokument</t>
-  </si>
-  <si>
-    <t>Testreport(?)</t>
-  </si>
-  <si>
     <t>Installationsanleitung</t>
   </si>
   <si>
     <t>Alle Seiten mit sinnvollem Inhalt gefüllt?</t>
+  </si>
+  <si>
+    <t>User Stories Dokument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja </t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>gecheckt am 17.06.16</t>
+  </si>
+  <si>
+    <t>nicht nötig</t>
+  </si>
+  <si>
+    <t>keine schachtelung nötig</t>
+  </si>
+  <si>
+    <t>nicht vorhanden</t>
+  </si>
+  <si>
+    <t>weder noch vorhanden</t>
+  </si>
+  <si>
+    <t>gecheckt am 17.06.2016</t>
   </si>
 </sst>
 </file>
@@ -429,22 +450,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G20"/>
+  <dimension ref="B1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="18.75">
+    <row r="1" spans="2:6" ht="18.75">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -453,155 +475,254 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7">
+    </row>
+    <row r="2" spans="2:6">
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="2:7">
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="2:7">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:7">
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="2:7">
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="2:7">
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="2:7">
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="2:7">
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:5">
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:6">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>

</xml_diff>

<commit_message>
checked architecture document, user stories doc and installation manual, also added document status entry
</commit_message>
<xml_diff>
--- a/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Dokumente.xlsx
+++ b/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Dokumente.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>Checkliste Dokumente</t>
   </si>
@@ -90,9 +90,6 @@
     <t xml:space="preserve">ja </t>
   </si>
   <si>
-    <t>nein</t>
-  </si>
-  <si>
     <t>gecheckt am 17.06.16</t>
   </si>
   <si>
@@ -109,6 +106,12 @@
   </si>
   <si>
     <t>gecheckt am 17.06.2016</t>
+  </si>
+  <si>
+    <t>Dokumentenstatus: final</t>
+  </si>
+  <si>
+    <t>Dokumentenstatus: to be reviewed</t>
   </si>
 </sst>
 </file>
@@ -453,16 +456,16 @@
   <dimension ref="B1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="54.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -576,7 +579,7 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -590,7 +593,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:6">
@@ -618,7 +621,7 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -660,7 +663,7 @@
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -674,7 +677,7 @@
         <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:6">
@@ -685,10 +688,10 @@
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -702,7 +705,7 @@
         <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -712,15 +715,22 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="1"/>

</xml_diff>